<commit_message>
Conditional Formatting Excel Tutorial File
Conditional Formatting Excel Tutorial File
</commit_message>
<xml_diff>
--- a/Conditional Formatting Excel Tutorial File.xlsx
+++ b/Conditional Formatting Excel Tutorial File.xlsx
@@ -1,24 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/579481080490e445/Documents/Excel Series Excels/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE12AABD-2C2A-4D60-B298-E861FD33474F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
     <sheet name="Sales" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -295,8 +289,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,7 +327,20 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -389,7 +396,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -441,7 +448,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -635,21 +642,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1027015F-D30F-450C-928C-DE78480974B7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -664,7 +671,7 @@
     <col min="11" max="11" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -699,7 +706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -734,7 +741,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -769,7 +776,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -804,7 +811,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -839,7 +846,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -874,7 +881,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -909,7 +916,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -944,7 +951,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -979,7 +986,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -1014,37 +1021,46 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:4">
       <c r="D22" t="str">
         <f t="shared" ref="D22:D23" si="0">CONCATENATE(B12," ",C12)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:4">
       <c r="D23" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CCAA7F-6F85-4102-B7D4-D80770622F9F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13">
       <c r="B1" t="s">
         <v>72</v>
       </c>
@@ -1082,7 +1098,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1123,7 +1139,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -1164,7 +1180,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -1206,6 +1222,30 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:M2">
+    <cfRule type="iconSet" priority="3">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:M3">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:M4">
+    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>